<commit_message>
added data and calculations for other years, updated README.md.
</commit_message>
<xml_diff>
--- a/processed_data.xlsx
+++ b/processed_data.xlsx
@@ -374,7 +374,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2014</t>
         </is>
       </c>
     </row>
@@ -388,7 +388,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>136960</v>
+        <v>65830</v>
       </c>
     </row>
     <row r="3">
@@ -400,7 +400,9 @@
           <t>Sales Growth</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>2.194e-07</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -412,7 +414,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>59550</v>
+        <v>25690</v>
       </c>
     </row>
     <row r="5">
@@ -425,7 +427,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>50510</v>
+        <v>20710</v>
       </c>
     </row>
     <row r="6">
@@ -438,7 +440,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9040</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="7">
@@ -451,7 +453,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8160</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="8">
@@ -464,7 +466,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>871</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="9">
@@ -476,7 +478,9 @@
           <t>COGS Growth</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>2.476e-07</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -488,7 +492,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>77410</v>
+        <v>40140</v>
       </c>
     </row>
     <row r="11">
@@ -500,7 +504,9 @@
           <t>Gross Income Growth</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>2.018e-07</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -523,7 +529,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>45880</v>
+        <v>23810</v>
       </c>
     </row>
     <row r="14">
@@ -536,7 +542,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>21420</v>
+        <v>9830</v>
       </c>
     </row>
     <row r="15">
@@ -549,7 +555,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>24460</v>
+        <v>13980</v>
       </c>
     </row>
     <row r="16">
@@ -561,7 +567,9 @@
           <t>SGA Growth</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>2.607e-07</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -584,7 +592,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>900</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19">
@@ -597,7 +605,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>30630</v>
+        <v>-281</v>
       </c>
     </row>
     <row r="20">
@@ -610,7 +618,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2640</v>
+        <v>570</v>
       </c>
     </row>
     <row r="21">
@@ -623,7 +631,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1880</v>
+        <v>746</v>
       </c>
     </row>
     <row r="22">
@@ -635,9 +643,7 @@
           <t>Equity in Affiliates (Pretax)</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>-120</v>
-      </c>
+      <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -649,7 +655,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24">
@@ -661,7 +667,9 @@
           <t>Interest Expense Growth</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>1.923e-07</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -673,7 +681,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>206</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
@@ -685,9 +693,7 @@
           <t>Interest Capitalized</t>
         </is>
       </c>
-      <c r="C26" t="n">
-        <v>92</v>
-      </c>
+      <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -699,7 +705,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>34910</v>
+        <v>17260</v>
       </c>
     </row>
     <row r="28">
@@ -711,7 +717,9 @@
           <t>Pretax Income Growth</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>2.289e-07</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -734,7 +742,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>4179.999999999999</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="31">
@@ -747,7 +755,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2150</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="32">
@@ -760,7 +768,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1250</v>
+        <v>774</v>
       </c>
     </row>
     <row r="33">
@@ -773,7 +781,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>907</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34">
@@ -786,7 +794,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-134</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="35">
@@ -832,7 +840,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>30740</v>
+        <v>13620</v>
       </c>
     </row>
     <row r="39">
@@ -856,7 +864,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>30740</v>
+        <v>13620</v>
       </c>
     </row>
     <row r="41">
@@ -868,7 +876,9 @@
           <t>Net Income Growth</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
+      <c r="C41" t="n">
+        <v>-3.499e-07</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -890,7 +900,9 @@
           <t>Extraordinaries &amp; Discontinued Operations</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" t="n">
+        <v>516</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -901,7 +913,9 @@
           <t>Extra Items &amp; Gain/Loss Sale Of Assets</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" t="n">
+        <v>740</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -923,7 +937,9 @@
           <t>Discontinued Operations</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
+      <c r="C46" t="n">
+        <v>-224</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -935,7 +951,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>30740</v>
+        <v>14140</v>
       </c>
     </row>
     <row r="48">
@@ -959,7 +975,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>30740</v>
+        <v>13400</v>
       </c>
     </row>
     <row r="50">
@@ -972,7 +988,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.422e-05</v>
+        <v>1.982e-05</v>
       </c>
     </row>
     <row r="51">
@@ -984,7 +1000,9 @@
           <t>EPS (Basic) Growth</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" t="n">
+        <v>-3.547e-07</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -996,7 +1014,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>695.14</v>
+        <v>675.9400000000001</v>
       </c>
     </row>
     <row r="53">
@@ -1009,7 +1027,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4.370000000000001e-05</v>
+        <v>1.95e-05</v>
       </c>
     </row>
     <row r="54">
@@ -1021,7 +1039,9 @@
           <t>EPS (Diluted) Growth</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
+      <c r="C54" t="n">
+        <v>-3.544e-07</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1033,7 +1053,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>703.29</v>
+        <v>687.0700000000001</v>
       </c>
     </row>
     <row r="56">
@@ -1046,7 +1066,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>40570</v>
+        <v>21300</v>
       </c>
     </row>
     <row r="57">
@@ -1058,7 +1078,9 @@
           <t>EBITDA Growth</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="n">
+        <v>2.735e-07</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1081,7 +1103,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>109140</v>
+        <v>64400.00000000001</v>
       </c>
     </row>
     <row r="60">
@@ -1094,7 +1116,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>16700</v>
+        <v>18350</v>
       </c>
     </row>
     <row r="61">
@@ -1107,7 +1129,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>92440</v>
+        <v>46050</v>
       </c>
     </row>
     <row r="62">
@@ -1119,7 +1141,9 @@
           <t>Cash &amp; Short Term Investments Growth</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>1.347e-07</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1131,7 +1155,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>4.688000000000001e-07</v>
+        <v>4.985e-07</v>
       </c>
     </row>
     <row r="64">
@@ -1144,7 +1168,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>21190</v>
+        <v>10850</v>
       </c>
     </row>
     <row r="65">
@@ -1157,7 +1181,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>20840</v>
+        <v>9380</v>
       </c>
     </row>
     <row r="66">
@@ -1170,7 +1194,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>21570</v>
+        <v>9610</v>
       </c>
     </row>
     <row r="67">
@@ -1183,7 +1207,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>-729</v>
+        <v>-225</v>
       </c>
     </row>
     <row r="68">
@@ -1196,7 +1220,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>355</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="69">
@@ -1208,7 +1232,9 @@
           <t>Accounts Receivable Growth</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>2.821e-07</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1220,7 +1246,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>6.46e-06</v>
+        <v>6.07e-06</v>
       </c>
     </row>
     <row r="71">
@@ -1232,9 +1258,7 @@
           <t>Inventories</t>
         </is>
       </c>
-      <c r="C71" t="n">
-        <v>1110</v>
-      </c>
+      <c r="C71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1245,9 +1269,7 @@
           <t>Finished Goods</t>
         </is>
       </c>
-      <c r="C72" t="n">
-        <v>1110</v>
-      </c>
+      <c r="C72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1292,7 +1314,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>4240</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="77">
@@ -1305,7 +1327,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>4240</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="78">
@@ -1318,7 +1340,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>135680</v>
+        <v>78660</v>
       </c>
     </row>
     <row r="79">
@@ -1331,7 +1353,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>59720</v>
+        <v>23880</v>
       </c>
     </row>
     <row r="80">
@@ -1344,7 +1366,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>82510</v>
+        <v>32750</v>
       </c>
     </row>
     <row r="81">
@@ -1357,7 +1379,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>30180</v>
+        <v>13330</v>
       </c>
     </row>
     <row r="82">
@@ -1381,7 +1403,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>30120</v>
+        <v>10920</v>
       </c>
     </row>
     <row r="84">
@@ -1394,7 +1416,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>5370</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="85">
@@ -1407,7 +1429,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>22790</v>
+        <v>8860</v>
       </c>
     </row>
     <row r="86">
@@ -1420,7 +1442,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>13860</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="87">
@@ -1432,9 +1454,7 @@
           <t>Other Long-Term Investments</t>
         </is>
       </c>
-      <c r="C87" t="n">
-        <v>12560</v>
-      </c>
+      <c r="C87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -1445,7 +1465,9 @@
           <t>Long-Term Note Receivable</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr"/>
+      <c r="C88" t="n">
+        <v>1330</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -1457,7 +1479,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>20110</v>
+        <v>20210</v>
       </c>
     </row>
     <row r="90">
@@ -1470,7 +1492,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>17890</v>
+        <v>15600</v>
       </c>
     </row>
     <row r="91">
@@ -1483,7 +1505,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2220</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="92">
@@ -1496,7 +1518,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2690</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="93">
@@ -1509,7 +1531,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>2690</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="94">
@@ -1522,7 +1544,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>232790</v>
+        <v>129190</v>
       </c>
     </row>
     <row r="95">
@@ -1534,7 +1556,9 @@
           <t>Assets - Total - Growth</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr"/>
+      <c r="C95" t="n">
+        <v>1.415e-07</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -1545,7 +1569,9 @@
           <t>ST Debt &amp; Current Portion LT Debt</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr"/>
+      <c r="C96" t="n">
+        <v>2010</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -1556,7 +1582,9 @@
           <t>Short Term Debt</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr"/>
+      <c r="C97" t="n">
+        <v>2000</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -1567,7 +1595,9 @@
           <t>Current Portion of Long Term Debt</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr"/>
+      <c r="C98" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -1579,7 +1609,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>4380</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="100">
@@ -1591,7 +1621,9 @@
           <t>Accounts Payable Growth</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr"/>
+      <c r="C100" t="n">
+        <v>5.37e-07</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -1603,7 +1635,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102">
@@ -1616,7 +1648,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>30170</v>
+        <v>12960</v>
       </c>
     </row>
     <row r="103">
@@ -1640,7 +1672,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>6840</v>
+        <v>3070</v>
       </c>
     </row>
     <row r="105">
@@ -1653,7 +1685,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>23330</v>
+        <v>9890</v>
       </c>
     </row>
     <row r="106">
@@ -1666,7 +1698,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>34620</v>
+        <v>16780</v>
       </c>
     </row>
     <row r="107">
@@ -1679,7 +1711,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>4010</v>
+        <v>3230</v>
       </c>
     </row>
     <row r="108">
@@ -1692,7 +1724,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>3950</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="109">
@@ -1705,7 +1737,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>3950</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="110">
@@ -1729,7 +1761,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>62</v>
+        <v>236</v>
       </c>
     </row>
     <row r="112">
@@ -1753,7 +1785,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>527</v>
+        <v>582</v>
       </c>
     </row>
     <row r="114">
@@ -1766,7 +1798,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1260</v>
+        <v>758</v>
       </c>
     </row>
     <row r="115">
@@ -1779,7 +1811,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>737</v>
+        <v>176</v>
       </c>
     </row>
     <row r="116">
@@ -1792,7 +1824,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>15270</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="117">
@@ -1805,7 +1837,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>14870</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="118">
@@ -1818,7 +1850,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>396</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119">
@@ -1831,7 +1863,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>55160</v>
+        <v>25330</v>
       </c>
     </row>
     <row r="120">
@@ -1855,7 +1887,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>2.37e-07</v>
+        <v>1.96e-07</v>
       </c>
     </row>
     <row r="122">
@@ -1901,7 +1933,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>177630</v>
+        <v>103860</v>
       </c>
     </row>
     <row r="126">
@@ -1914,7 +1946,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.695556</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="127">
@@ -1927,7 +1959,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>134890</v>
+        <v>75070</v>
       </c>
     </row>
     <row r="128">
@@ -1951,7 +1983,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>-1880</v>
+        <v>-980</v>
       </c>
     </row>
     <row r="130">
@@ -1964,7 +1996,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>-688</v>
+        <v>421</v>
       </c>
     </row>
     <row r="131">
@@ -1999,7 +2031,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>7.63e-07</v>
+        <v>8.040000000000001e-07</v>
       </c>
     </row>
     <row r="134">
@@ -2012,7 +2044,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>177630</v>
+        <v>103860</v>
       </c>
     </row>
     <row r="135">
@@ -2025,7 +2057,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>7.63e-07</v>
+        <v>8.040000000000001e-07</v>
       </c>
     </row>
     <row r="136">
@@ -2049,7 +2081,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>177630</v>
+        <v>103860</v>
       </c>
     </row>
     <row r="138">
@@ -2062,7 +2094,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>232790</v>
+        <v>129190</v>
       </c>
     </row>
     <row r="139">
@@ -2075,7 +2107,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>30740</v>
+        <v>14140</v>
       </c>
     </row>
     <row r="140">
@@ -2087,7 +2119,9 @@
           <t>Net Income Growth</t>
         </is>
       </c>
-      <c r="C140" t="inlineStr"/>
+      <c r="C140" t="n">
+        <v>-3.499e-07</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -2099,7 +2133,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>9040</v>
+        <v>4980</v>
       </c>
     </row>
     <row r="142">
@@ -2112,7 +2146,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>8160</v>
+        <v>3520</v>
       </c>
     </row>
     <row r="143">
@@ -2125,7 +2159,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>871</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="144">
@@ -2138,7 +2172,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>778</v>
+        <v>-104</v>
       </c>
     </row>
     <row r="145">
@@ -2151,7 +2185,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>778</v>
+        <v>-104</v>
       </c>
     </row>
     <row r="146">
@@ -2175,7 +2209,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>2510</v>
+        <v>2690</v>
       </c>
     </row>
     <row r="148">
@@ -2188,7 +2222,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>43060</v>
+        <v>21700</v>
       </c>
     </row>
     <row r="149">
@@ -2212,7 +2246,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>4910</v>
+        <v>672</v>
       </c>
     </row>
     <row r="151">
@@ -2225,7 +2259,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>-2170</v>
+        <v>-1640</v>
       </c>
     </row>
     <row r="152">
@@ -2238,7 +2272,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>1070</v>
+        <v>436</v>
       </c>
     </row>
     <row r="153">
@@ -2251,7 +2285,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>-836</v>
+        <v>284</v>
       </c>
     </row>
     <row r="154">
@@ -2264,7 +2298,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>47970</v>
+        <v>22380</v>
       </c>
     </row>
     <row r="155">
@@ -2276,7 +2310,9 @@
           <t>Net Operating Cash Flow Growth</t>
         </is>
       </c>
-      <c r="C155" t="inlineStr"/>
+      <c r="C155" t="n">
+        <v>3.562e-07</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -2288,7 +2324,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>3.503e-07</v>
+        <v>3.399e-07</v>
       </c>
     </row>
     <row r="157">
@@ -2301,7 +2337,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>-25140</v>
+        <v>-10960</v>
       </c>
     </row>
     <row r="158">
@@ -2314,7 +2350,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>-25140</v>
+        <v>-10960</v>
       </c>
     </row>
     <row r="159">
@@ -2337,7 +2373,9 @@
           <t>Capital Expenditures Growth</t>
         </is>
       </c>
-      <c r="C160" t="inlineStr"/>
+      <c r="C160" t="n">
+        <v>9.210000000000001e-08</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -2349,7 +2387,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>-1.836e-07</v>
+        <v>-1.665e-07</v>
       </c>
     </row>
     <row r="162">
@@ -2362,7 +2400,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>-1490</v>
+        <v>-4890</v>
       </c>
     </row>
     <row r="163">
@@ -2375,7 +2413,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>98</v>
+        <v>386</v>
       </c>
     </row>
     <row r="164">
@@ -2388,7 +2426,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>-1970</v>
+        <v>-7000</v>
       </c>
     </row>
     <row r="165">
@@ -2401,7 +2439,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>-52230</v>
+        <v>-58310</v>
       </c>
     </row>
     <row r="166">
@@ -2414,7 +2452,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>50260</v>
+        <v>51320</v>
       </c>
     </row>
     <row r="167">
@@ -2437,7 +2475,9 @@
           <t>Other Sources</t>
         </is>
       </c>
-      <c r="C168" t="inlineStr"/>
+      <c r="C168" t="n">
+        <v>1400</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -2449,7 +2489,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>-28500</v>
+        <v>-21060</v>
       </c>
     </row>
     <row r="170">
@@ -2461,7 +2501,9 @@
           <t>Net Investing Cash Flow Growth</t>
         </is>
       </c>
-      <c r="C170" t="inlineStr"/>
+      <c r="C170" t="n">
+        <v>-1.261e-07</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -2473,7 +2515,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>-2.081e-07</v>
+        <v>-3.198e-07</v>
       </c>
     </row>
     <row r="172">
@@ -2518,9 +2560,7 @@
           <t>Change in Capital Stock</t>
         </is>
       </c>
-      <c r="C175" t="n">
-        <v>-9080</v>
-      </c>
+      <c r="C175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -2531,9 +2571,7 @@
           <t>Repurchase of Common &amp; Preferred Stk.</t>
         </is>
       </c>
-      <c r="C176" t="n">
-        <v>-9080</v>
-      </c>
+      <c r="C176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -2578,7 +2616,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>-61</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="181">
@@ -2602,7 +2640,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>-61</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="183">
@@ -2615,7 +2653,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6770</v>
+        <v>11630</v>
       </c>
     </row>
     <row r="184">
@@ -2628,7 +2666,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>-6830</v>
+        <v>-11640</v>
       </c>
     </row>
     <row r="185">
@@ -2641,7 +2679,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>-4040</v>
+        <v>-1420</v>
       </c>
     </row>
     <row r="186">
@@ -2654,7 +2692,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>-4990</v>
+        <v>-2070</v>
       </c>
     </row>
     <row r="187">
@@ -2667,7 +2705,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>950</v>
+        <v>648</v>
       </c>
     </row>
     <row r="188">
@@ -2680,7 +2718,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>-13180</v>
+        <v>-1440</v>
       </c>
     </row>
     <row r="189">
@@ -2692,7 +2730,9 @@
           <t>Net Financing Cash Flow Growth</t>
         </is>
       </c>
-      <c r="C189" t="inlineStr"/>
+      <c r="C189" t="n">
+        <v>-1.9361e-06</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -2704,7 +2744,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>-9.619999999999999e-08</v>
+        <v>-2.19e-08</v>
       </c>
     </row>
     <row r="191">
@@ -2717,7 +2757,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>-302</v>
+        <v>-433</v>
       </c>
     </row>
     <row r="192">
@@ -2741,7 +2781,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>5990</v>
+        <v>-551</v>
       </c>
     </row>
     <row r="194">
@@ -2754,7 +2794,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>22830</v>
+        <v>11420</v>
       </c>
     </row>
     <row r="195">
@@ -2766,7 +2806,9 @@
           <t>Free Cash Flow Growth</t>
         </is>
       </c>
-      <c r="C195" t="inlineStr"/>
+      <c r="C195" t="n">
+        <v>4.559000000000001e-07</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">

</xml_diff>